<commit_message>
TS 1.4 Input and other edits 11/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Rule Processing Table.xlsx
+++ b/TS Jatai Working/Raja Files/Rule Processing Table.xlsx
@@ -3495,13 +3495,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -3675,74 +3681,74 @@
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4026,7 +4032,7 @@
   <dimension ref="A3:V306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="I15" sqref="I15"/>

</xml_diff>